<commit_message>
psa talk and june repro
</commit_message>
<xml_diff>
--- a/kelp_reproductive_timing.xlsx
+++ b/kelp_reproductive_timing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B3BB811-C9A7-4A62-9EB2-142A7571F3BF}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEB8AB29-3D34-4F6F-9FC6-A7355671FE16}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>year</t>
   </si>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>Nereocystis.luetkeana</t>
+  </si>
+  <si>
+    <t>Alaria.marginata</t>
+  </si>
+  <si>
+    <t>Costaria.costata</t>
   </si>
   <si>
     <t>y</t>
@@ -105,6 +112,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,7 +393,7 @@
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,8 +409,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2022</v>
       </c>
@@ -410,10 +427,10 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2022</v>
       </c>
@@ -424,10 +441,10 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -435,7 +452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -446,10 +463,10 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -460,10 +477,10 @@
         <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2022</v>
       </c>
@@ -474,10 +491,10 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2022</v>
       </c>
@@ -488,10 +505,10 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2022</v>
       </c>
@@ -502,10 +519,10 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2023</v>
       </c>
@@ -516,7 +533,41 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2023</v>
+      </c>
+      <c r="B11">
         <v>5</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2023</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tidal quadrat height code
</commit_message>
<xml_diff>
--- a/kelp_reproductive_timing.xlsx
+++ b/kelp_reproductive_timing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{647CA32B-02C1-46F5-9E9D-1DE353141697}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A65B6F1-FBDD-48E6-97C7-09BE8E00198F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>year</t>
   </si>
@@ -377,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,6 +569,37 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2023</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2023</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
nov 2023 data, repro time search
</commit_message>
<xml_diff>
--- a/kelp_reproductive_timing.xlsx
+++ b/kelp_reproductive_timing.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FEE6E68-B9B1-4073-861D-1A4150AE10BC}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AFF3FB6-52A5-42B3-99BD-01483FE0CFAB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -58,6 +59,15 @@
   <si>
     <t>costaria_costata</t>
   </si>
+  <si>
+    <t>type_of_data</t>
+  </si>
+  <si>
+    <t>presence_abscence</t>
+  </si>
+  <si>
+    <t>time_search</t>
+  </si>
 </sst>
 </file>
 
@@ -72,12 +82,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,11 +391,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,6 +663,394 @@
         <v>1</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2023</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF41119-B066-416B-9FED-8411F55EBD68}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" customWidth="1"/>
+    <col min="7" max="8" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2022</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2022</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2022</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2022</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2022</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2022</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2022</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2023</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2023</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2023</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2023</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2023</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2023</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2023</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2023</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2023</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B21" s="1">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1">
+        <v>203</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
hieight fix and paper edits
</commit_message>
<xml_diff>
--- a/kelp_reproductive_timing.xlsx
+++ b/kelp_reproductive_timing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AFF3FB6-52A5-42B3-99BD-01483FE0CFAB}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E927128-D467-4C98-BBC0-10E1BE13108E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -73,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,18 +82,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,7 +104,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,15 +392,15 @@
       <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +423,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>2022</v>
       </c>
@@ -443,7 +437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2022</v>
       </c>
@@ -457,7 +451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -468,7 +462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -482,7 +476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -490,7 +484,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>2022</v>
       </c>
@@ -504,7 +498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>2022</v>
       </c>
@@ -518,7 +512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>2022</v>
       </c>
@@ -532,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>2022</v>
       </c>
@@ -546,7 +540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>2023</v>
       </c>
@@ -554,7 +548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>2023</v>
       </c>
@@ -568,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>2023</v>
       </c>
@@ -576,7 +570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>2023</v>
       </c>
@@ -584,7 +578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -601,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>2023</v>
       </c>
@@ -618,7 +612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2023</v>
       </c>
@@ -632,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2023</v>
       </c>
@@ -649,7 +643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2023</v>
       </c>
@@ -663,7 +657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2023</v>
       </c>
@@ -681,23 +675,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF41119-B066-416B-9FED-8411F55EBD68}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="8" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>2022</v>
       </c>
@@ -736,11 +731,20 @@
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
       <c r="H2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2022</v>
       </c>
@@ -750,14 +754,23 @@
       <c r="C3">
         <v>19</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
       <c r="H3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -767,11 +780,23 @@
       <c r="C4">
         <v>15</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
       <c r="H4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -781,25 +806,49 @@
       <c r="C5">
         <v>14</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
       <c r="E5">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
       <c r="H5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>2022</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
+      <c r="C6">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
       <c r="H6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>2022</v>
       </c>
@@ -809,14 +858,23 @@
       <c r="C7">
         <v>23</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
       <c r="H7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>2022</v>
       </c>
@@ -829,11 +887,20 @@
       <c r="D8">
         <v>1</v>
       </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
       <c r="H8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>2022</v>
       </c>
@@ -846,11 +913,20 @@
       <c r="D9">
         <v>1</v>
       </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
       <c r="H9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>2022</v>
       </c>
@@ -863,22 +939,46 @@
       <c r="D10">
         <v>1</v>
       </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
       <c r="H10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>2023</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
       <c r="H11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>2023</v>
       </c>
@@ -891,33 +991,72 @@
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
       <c r="H12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>2023</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
+      <c r="C13">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
       <c r="H13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>2023</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
       <c r="H14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -933,11 +1072,17 @@
       <c r="E15">
         <v>1</v>
       </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
       <c r="H15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>2023</v>
       </c>
@@ -953,11 +1098,17 @@
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
       <c r="H16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>2023</v>
       </c>
@@ -967,14 +1118,23 @@
       <c r="C17">
         <v>4</v>
       </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
       <c r="E17">
         <v>1</v>
       </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
       <c r="H17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>2023</v>
       </c>
@@ -990,11 +1150,17 @@
       <c r="E18">
         <v>1</v>
       </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
       <c r="H18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>2023</v>
       </c>
@@ -1007,11 +1173,20 @@
       <c r="D19">
         <v>1</v>
       </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
       <c r="H19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>2023</v>
       </c>
@@ -1021,11 +1196,23 @@
       <c r="C20">
         <v>20</v>
       </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
       <c r="H20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="1" customFormat="1">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -1048,6 +1235,32 @@
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B22" s="1">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>289</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added image to app
</commit_message>
<xml_diff>
--- a/kelp_reproductive_timing.xlsx
+++ b/kelp_reproductive_timing.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E927128-D467-4C98-BBC0-10E1BE13108E}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F441693E-B299-4ABD-89E6-FE95121710E3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -73,7 +72,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,9 +101,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,315 +382,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
-  <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
-        <v>2022</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>2022</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>19</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>2022</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>2022</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>2022</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>2022</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>23</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>2022</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>13</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>2022</v>
-      </c>
-      <c r="B9">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>27</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>2022</v>
-      </c>
-      <c r="B10">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>25</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>2023</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
-        <v>2023</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>18</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>2023</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>2023</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
-        <v>2023</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>8</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
-        <v>2023</v>
-      </c>
-      <c r="B16">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>2023</v>
-      </c>
-      <c r="B17">
-        <v>7</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
-        <v>2023</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
-        <v>2023</v>
-      </c>
-      <c r="B19">
-        <v>9</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20">
-        <v>2023</v>
-      </c>
-      <c r="B20">
-        <v>10</v>
-      </c>
-      <c r="C20">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF41119-B066-416B-9FED-8411F55EBD68}">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="8" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -718,7 +426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2022</v>
       </c>
@@ -744,7 +452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2022</v>
       </c>
@@ -770,7 +478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -796,7 +504,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -822,7 +530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -848,7 +556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2022</v>
       </c>
@@ -874,7 +582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2022</v>
       </c>
@@ -900,7 +608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2022</v>
       </c>
@@ -926,7 +634,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2022</v>
       </c>
@@ -952,7 +660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2023</v>
       </c>
@@ -978,7 +686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2023</v>
       </c>
@@ -1004,7 +712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2023</v>
       </c>
@@ -1030,7 +738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2023</v>
       </c>
@@ -1056,7 +764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -1082,7 +790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2023</v>
       </c>
@@ -1108,7 +816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2023</v>
       </c>
@@ -1134,7 +842,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2023</v>
       </c>
@@ -1160,7 +868,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2023</v>
       </c>
@@ -1186,7 +894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2023</v>
       </c>
@@ -1212,40 +920,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1">
-      <c r="A21" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B21" s="1">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2023</v>
+      </c>
+      <c r="B21">
         <v>11</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>17</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>203</v>
       </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1" t="s">
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B22" s="1">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2023</v>
+      </c>
+      <c r="B22">
         <v>12</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>12</v>
       </c>
       <c r="D22">

</xml_diff>

<commit_message>
overrite of biodiv analysis script
</commit_message>
<xml_diff>
--- a/kelp_reproductive_timing.xlsx
+++ b/kelp_reproductive_timing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFB18DFE-ECED-4E0F-AE0F-77FD9630060B}"/>
+  <xr:revisionPtr revIDLastSave="217" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11E50D4C-B095-4BB9-AF5D-631FD671B1EA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -383,11 +383,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF41119-B066-416B-9FED-8411F55EBD68}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,6 +1050,136 @@
         <v>9</v>
       </c>
     </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2024</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2024</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2024</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2024</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>21</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2024</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>22</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
submission and sept 2024 transects
</commit_message>
<xml_diff>
--- a/kelp_reproductive_timing.xlsx
+++ b/kelp_reproductive_timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B0C671F-2CCD-4AE6-BC33-9A64E795D95A}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AECBA6A6-D130-4CDB-A277-2CE7BA8AAA0C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -383,11 +383,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF41119-B066-416B-9FED-8411F55EBD68}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,6 +1206,32 @@
         <v>8</v>
       </c>
     </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2024</v>
+      </c>
+      <c r="B32">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>16</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>